<commit_message>
datos nuevos para testear
</commit_message>
<xml_diff>
--- a/data/FinishedTable/ExcelConDatosNuevos.xlsx
+++ b/data/FinishedTable/ExcelConDatosNuevos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,213 +24,213 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Land km2</t>
-  </si>
-  <si>
-    <t>Forest Cover (%)</t>
-  </si>
-  <si>
-    <t>Average Temp (C)</t>
-  </si>
-  <si>
-    <t>Average elevation</t>
-  </si>
-  <si>
-    <t>Difference elevation</t>
-  </si>
-  <si>
-    <t>% that is Public Land</t>
-  </si>
-  <si>
-    <t>% that is Private Land</t>
-  </si>
-  <si>
-    <t>Average Wind Speed (mph)</t>
-  </si>
-  <si>
-    <t>Installed Wind Capacity (MW)</t>
-  </si>
-  <si>
-    <t>Nuclear Year to Date (MW/h)</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Pais</t>
-  </si>
-  <si>
-    <t>España</t>
-  </si>
-  <si>
-    <t>Francia</t>
-  </si>
-  <si>
-    <t>Alemania</t>
-  </si>
-  <si>
-    <t>Inglaterra</t>
-  </si>
-  <si>
-    <t>Greece</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land km2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Cover (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Temp (C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average elevation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference elevation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% that is Public Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% that is Private Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Wind Speed (mph)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed Wind Capacity (MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuclear Year to Date (MW/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alabama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alaska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkansas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connecticut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delaware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idaho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kansas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kentucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louisiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maryland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massachusetts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minnesota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mississippi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missouri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebraska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Hampshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Jersey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Carolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Dakota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ohio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oklahoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oregon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pennsylvania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhode Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Carolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Dakota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennessee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vermont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wisconsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyoming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alemania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inglaterra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -352,18 +352,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.306976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.4666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,20 +2317,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4232558139535"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,19 +2359,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>64</v>
       </c>
@@ -2384,8 +2384,20 @@
       <c r="E2" s="0" t="n">
         <v>660</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="n">
+        <v>3718</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>23025</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>54740</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>65</v>
       </c>
@@ -2401,8 +2413,20 @@
       <c r="E3" s="0" t="n">
         <v>375</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0" t="n">
+        <v>4810</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>10358</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>416800</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>66</v>
       </c>
@@ -2418,8 +2442,20 @@
       <c r="E4" s="0" t="n">
         <v>263</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>2962</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>44947</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>86810.32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>67</v>
       </c>
@@ -2435,8 +2471,20 @@
       <c r="E5" s="0" t="n">
         <v>162</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="n">
+        <v>1344</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>13603</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>63894.54</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>68</v>
       </c>
@@ -2451,6 +2499,18 @@
       </c>
       <c r="E6" s="0" t="n">
         <v>498</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2919</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>2152</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>